<commit_message>
updated API commands examples
</commit_message>
<xml_diff>
--- a/OCS-900N API Commands.xlsx
+++ b/OCS-900N API Commands.xlsx
@@ -5,21 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atlonainc10-my.sharepoint.com/personal/joshua_small_atlona_com/Documents/PRD/AT-OCS-900N/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\AT-OCS-900N\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="591" documentId="8_{C27AE798-CD5E-44DD-B182-E209D2A5C34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{109608A7-1DD1-40F7-BAAB-04F693BB4570}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BD6389-BF1F-4A26-B53C-DC4F46A8D8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="1920" windowWidth="8115" windowHeight="15555" firstSheet="2" activeTab="3" xr2:uid="{0EED16D4-E153-423C-AD5A-DC2EE445FF9D}"/>
+    <workbookView xWindow="1065" yWindow="1920" windowWidth="8115" windowHeight="15555" xr2:uid="{0EED16D4-E153-423C-AD5A-DC2EE445FF9D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Get" sheetId="2" r:id="rId2"/>
-    <sheet name="Set" sheetId="3" r:id="rId3"/>
-    <sheet name="Variables" sheetId="7" r:id="rId4"/>
-    <sheet name="Methods" sheetId="4" r:id="rId5"/>
-    <sheet name="ID" sheetId="5" r:id="rId6"/>
-    <sheet name="Error" sheetId="6" r:id="rId7"/>
+    <sheet name="Get" sheetId="2" r:id="rId1"/>
+    <sheet name="Set" sheetId="3" r:id="rId2"/>
+    <sheet name="Methods" sheetId="4" r:id="rId3"/>
+    <sheet name="ID" sheetId="5" r:id="rId4"/>
+    <sheet name="Error" sheetId="6" r:id="rId5"/>
+    <sheet name="Velocity" sheetId="7" r:id="rId6"/>
+    <sheet name="textjoin" sheetId="1" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="189">
   <si>
     <t>get</t>
   </si>
@@ -1051,13 +1051,6 @@
   </si>
   <si>
     <t>{
-  "motion": {
-    "lastDetection": "49710:06:28:1"
-  }
-}</t>
-  </si>
-  <si>
-    <t>{
   "temperature": {
     "values": {
      "F": 72.0
@@ -1112,23 +1105,48 @@
     }
   }
 }</t>
+  </si>
+  <si>
+    <t>Variable Value</t>
+  </si>
+  <si>
+    <t>{
+  "motion": {
+    "lastDetection": "1:06:28:1"
+  }
+}</t>
+  </si>
+  <si>
+    <t>1:06:28:1</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Cascadia Code PL"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Cascadia Code PL"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1163,6 +1181,27 @@
       <name val="Cascadia Code PL"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Cascadia Code PL"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Cascadia Code PL"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cascadia Code PL"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1184,7 +1223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -1194,40 +1233,127 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="30">
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
+        <sz val="12"/>
         <color theme="1"/>
         <name val="Cascadia Code PL"/>
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Cascadia Code PL"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Cascadia Code PL"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Cascadia Code PL"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Cascadia Code PL"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1238,7 +1364,7 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1258,25 +1384,6 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Cascadia Code PL"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1310,22 +1417,33 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Cascadia Code PL"/>
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Cascadia Code PL"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1386,30 +1504,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Cascadia Code PL"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1417,29 +1512,10 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Cascadia Code PL"/>
-        <family val="3"/>
-        <scheme val="none"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Cascadia Code PL"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1451,28 +1527,25 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Cascadia Code PL"/>
-        <family val="3"/>
-        <scheme val="none"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Cascadia Code PL"/>
-        <family val="3"/>
-        <scheme val="none"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1552,7 +1625,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1561,13 +1634,13 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Cascadia Code PL"/>
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1605,11 +1678,15 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1620,10 +1697,11 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1632,13 +1710,13 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Cascadia Code PL"/>
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1695,10 +1773,10 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Atlona" pivot="0" count="4" xr9:uid="{F9B6A13A-134A-4369-AD64-87B8D77E3B45}">
-      <tableStyleElement type="wholeTable" dxfId="27"/>
-      <tableStyleElement type="headerRow" dxfId="26"/>
-      <tableStyleElement type="firstRowStripe" dxfId="25"/>
-      <tableStyleElement type="secondRowStripe" dxfId="24"/>
+      <tableStyleElement type="wholeTable" dxfId="29"/>
+      <tableStyleElement type="headerRow" dxfId="28"/>
+      <tableStyleElement type="firstRowStripe" dxfId="27"/>
+      <tableStyleElement type="secondRowStripe" dxfId="26"/>
     </tableStyle>
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{47E70D94-5E5A-41E2-A443-10D7AF127A13}"/>
   </tableStyles>
@@ -1714,75 +1792,77 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33F869EC-2C68-497D-9D0C-3F4510D465F5}" name="Get" displayName="Get" ref="A1:B15" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33F869EC-2C68-497D-9D0C-3F4510D465F5}" name="Get" displayName="Get" ref="A1:B15" totalsRowShown="0" headerRowDxfId="0" dataDxfId="14">
   <autoFilter ref="A1:B15" xr:uid="{33F869EC-2C68-497D-9D0C-3F4510D465F5}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7A5B13B4-EA33-48DF-9861-93F992C1FCBA}" name="Get Request" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{766450EB-4539-4E52-B4BF-ED78A02B6DDF}" name="Get Reply" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{7A5B13B4-EA33-48DF-9861-93F992C1FCBA}" name="Get Request" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{766450EB-4539-4E52-B4BF-ED78A02B6DDF}" name="Get Reply" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="Atlona" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E56A572-36A0-4332-B926-FE69928C5D93}" name="Set" displayName="Set" ref="A1:C13" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E56A572-36A0-4332-B926-FE69928C5D93}" name="Set" displayName="Set" ref="A1:C13" totalsRowShown="0" headerRowDxfId="1" dataDxfId="17">
   <autoFilter ref="A1:C13" xr:uid="{6E56A572-36A0-4332-B926-FE69928C5D93}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{317E6D25-5105-49DB-AE93-6D362339D790}" name="Set Request" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{6F54A2EF-B93E-46C0-B92B-65477D3E0A7F}" name="Set Example" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{FF1EA774-5C67-4BCE-AC33-24FBCC42EA50}" name="Set Example Reply" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{317E6D25-5105-49DB-AE93-6D362339D790}" name="Set Request" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{6F54A2EF-B93E-46C0-B92B-65477D3E0A7F}" name="Set Example" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{FF1EA774-5C67-4BCE-AC33-24FBCC42EA50}" name="Set Example Reply" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="Atlona" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BF568B31-D8B1-4856-ADC3-21C1699FBC90}" name="Variables" displayName="Variables" ref="A1:B9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:B9" xr:uid="{BF568B31-D8B1-4856-ADC3-21C1699FBC90}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D7D42A0F-8DB9-4B3C-A4D1-F73651E87E17}" name="Methods" displayName="Methods" ref="A1:B8" totalsRowShown="0" headerRowDxfId="2" dataDxfId="21">
+  <autoFilter ref="A1:B8" xr:uid="{D7D42A0F-8DB9-4B3C-A4D1-F73651E87E17}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{79C24783-B69A-4883-B4B1-3CC5E6616A08}" name="Variable Name" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{B468BAFC-DC1E-435F-AD59-C2BBA8834ADD}" name="Example Data" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{1D0FA7C7-0912-4FA5-8B9A-36E8D5B2B620}" name="Method Request" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{B70E94AE-5022-41BC-9A49-3FCFC3322D76}" name="Method Reply" dataDxfId="22"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="Atlona" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D7D42A0F-8DB9-4B3C-A4D1-F73651E87E17}" name="Methods" displayName="Methods" ref="A1:B8" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:B8" xr:uid="{D7D42A0F-8DB9-4B3C-A4D1-F73651E87E17}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B1BFF974-B937-4BAB-9D9B-74D1782E984C}" name="ID" displayName="ID" ref="A1:B2" totalsRowShown="0" headerRowDxfId="3" dataDxfId="11">
+  <autoFilter ref="A1:B2" xr:uid="{B1BFF974-B937-4BAB-9D9B-74D1782E984C}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1D0FA7C7-0912-4FA5-8B9A-36E8D5B2B620}" name="Method Request" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{B70E94AE-5022-41BC-9A49-3FCFC3322D76}" name="Method Reply" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{BFCE05DF-C728-41BA-8915-D5637D404020}" name="ID Example" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{BFC85FFA-2F7C-4076-AE7F-990A705414E7}" name="ID Example Reply" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="Atlona" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B1BFF974-B937-4BAB-9D9B-74D1782E984C}" name="ID" displayName="ID" ref="A1:B2" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:B2" xr:uid="{B1BFF974-B937-4BAB-9D9B-74D1782E984C}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BFCE05DF-C728-41BA-8915-D5637D404020}" name="ID Example" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{BFC85FFA-2F7C-4076-AE7F-990A705414E7}" name="ID Example Reply" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CA3665BD-EE91-49A2-87C2-4D4FAEC78F80}" name="Errors" displayName="Errors" ref="A1:A2" totalsRowShown="0" headerRowDxfId="4" dataDxfId="25">
+  <autoFilter ref="A1:A2" xr:uid="{CA3665BD-EE91-49A2-87C2-4D4FAEC78F80}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{639DD3CB-948C-49A1-9CF4-2D6C7B597741}" name="Error Reply" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="Atlona" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CA3665BD-EE91-49A2-87C2-4D4FAEC78F80}" name="Errors" displayName="Errors" ref="A1:A2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:A2" xr:uid="{CA3665BD-EE91-49A2-87C2-4D4FAEC78F80}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{639DD3CB-948C-49A1-9CF4-2D6C7B597741}" name="Error Reply" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BF568B31-D8B1-4856-ADC3-21C1699FBC90}" name="Variables" displayName="Variables" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
+  <autoFilter ref="A1:D9" xr:uid="{BF568B31-D8B1-4856-ADC3-21C1699FBC90}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{79C24783-B69A-4883-B4B1-3CC5E6616A08}" name="Variable Name" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B468BAFC-DC1E-435F-AD59-C2BBA8834ADD}" name="Example Data" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{F712ACE1-0732-4746-8D21-C4C408A8B60A}" name="Data Type" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{94605155-A5D1-4E86-B5E7-3B205BED259C}" name="Variable Value" dataDxfId="7"/>
   </tableColumns>
-  <tableStyleInfo name="Atlona" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Atlona">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Atlona Code">
   <a:themeElements>
-    <a:clrScheme name="Custom 1">
+    <a:clrScheme name="Atlona">
       <a:dk1>
         <a:srgbClr val="111111"/>
       </a:dk1>
@@ -1814,20 +1894,20 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="004976"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Atlona">
+    <a:fontScheme name="Atlona Code">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
+        <a:latin typeface="Cascadia Code PL"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
+        <a:latin typeface="Cascadia Code PL"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -1981,6 +2061,617 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23925345-A8BE-4B4F-959F-C9FE5268EEB4}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9AA4E1F-55D2-4C8A-AC7E-8CB31EF8CDA3}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="101.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="242.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="128.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="270.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="114" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="313.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="114" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="156.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="156.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="213.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="270.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="270.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="128.25" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523657EB-CA37-4493-B4B4-F0F4131A16FB}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="92.88671875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="99.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="270.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A8F835-FA33-4DA5-83B5-C81996F7BF5E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="101.77734375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178ACD6D-9418-44D7-900C-0A5B9E82BCD0}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="57" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9758462A-C110-4E0C-A116-5784E0114A4A}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="71.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="71.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="99.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" s="7">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="99.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="7">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="99.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="7">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="99.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="99.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" s="7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="99.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" s="7">
+        <v>22.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD736396-7576-45D9-956B-39CB84D93E24}">
   <dimension ref="A1:S36"/>
   <sheetViews>
@@ -1990,14 +2681,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="7.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.75" style="1" customWidth="1"/>
-    <col min="7" max="9" width="7.75" style="1" customWidth="1"/>
-    <col min="10" max="10" width="69.25" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="1"/>
+    <col min="1" max="2" width="7.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
+    <col min="7" max="9" width="7.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="69.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2981,577 +3672,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23925345-A8BE-4B4F-959F-C9FE5268EEB4}">
-  <dimension ref="A1:C17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="43.25" style="3" customWidth="1"/>
-    <col min="2" max="2" width="53.75" style="3" customWidth="1"/>
-    <col min="3" max="3" width="4" style="3" customWidth="1"/>
-    <col min="4" max="4" width="32.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="47" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="3"/>
-    <col min="8" max="8" width="32.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="3:3" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="C17" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9AA4E1F-55D2-4C8A-AC7E-8CB31EF8CDA3}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="101.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="47" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="242.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="270.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="114" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="313.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="114" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="156.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="156.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="213.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="270.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="270.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9758462A-C110-4E0C-A116-5784E0114A4A}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.25" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.75" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.625" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:3" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523657EB-CA37-4493-B4B4-F0F4131A16FB}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="92.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="57" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="57" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="57" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="285" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A8F835-FA33-4DA5-83B5-C81996F7BF5E}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="101.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178ACD6D-9418-44D7-900C-0A5B9E82BCD0}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="37.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>